<commit_message>
Updated panelApp panels to contain time_taken for metadata purposes
</commit_message>
<xml_diff>
--- a/data/panelapp/au/Achromatopsia.xlsx
+++ b/data/panelapp/au/Achromatopsia.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>panel</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>time_taken</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -479,6 +484,11 @@
           <t>Achromatopsia</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2021-10-05 10:49:56.144873</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -504,6 +514,11 @@
           <t>Achromatopsia</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2021-10-05 10:49:56.144884</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -529,6 +544,11 @@
           <t>Achromatopsia</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2021-10-05 10:49:56.144888</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -554,6 +574,11 @@
           <t>Achromatopsia</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2021-10-05 10:49:56.144890</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -579,6 +604,11 @@
           <t>Achromatopsia</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2021-10-05 10:49:56.144893</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -604,6 +634,11 @@
           <t>Achromatopsia</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2021-10-05 10:49:56.144896</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -629,6 +664,11 @@
           <t>Achromatopsia</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2021-10-05 10:49:56.144899</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -652,6 +692,11 @@
       <c r="E9" t="inlineStr">
         <is>
           <t>Achromatopsia</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2021-10-05 10:49:56.144901</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refined metadata to be additional tab
</commit_message>
<xml_diff>
--- a/data/panelapp/au/Achromatopsia.xlsx
+++ b/data/panelapp/au/Achromatopsia.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="metadata" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -486,7 +487,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2021-10-05 10:49:56.144873</t>
+          <t>2021-10-05 14:33:03.266002</t>
         </is>
       </c>
     </row>
@@ -516,7 +517,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2021-10-05 10:49:56.144884</t>
+          <t>2021-10-05 14:33:03.266010</t>
         </is>
       </c>
     </row>
@@ -546,7 +547,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2021-10-05 10:49:56.144888</t>
+          <t>2021-10-05 14:33:03.266013</t>
         </is>
       </c>
     </row>
@@ -576,7 +577,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2021-10-05 10:49:56.144890</t>
+          <t>2021-10-05 14:33:03.266016</t>
         </is>
       </c>
     </row>
@@ -606,7 +607,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2021-10-05 10:49:56.144893</t>
+          <t>2021-10-05 14:33:03.266019</t>
         </is>
       </c>
     </row>
@@ -636,7 +637,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2021-10-05 10:49:56.144896</t>
+          <t>2021-10-05 14:33:03.266021</t>
         </is>
       </c>
     </row>
@@ -666,7 +667,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2021-10-05 10:49:56.144899</t>
+          <t>2021-10-05 14:33:03.266024</t>
         </is>
       </c>
     </row>
@@ -696,7 +697,91 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2021-10-05 10:49:56.144901</t>
+          <t>2021-10-05 14:33:03.266026</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>data_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>data_id</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>data_version</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>data_version_created</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>panel_query_time</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>panel_get_request</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Achromatopsia</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>3149</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1.3</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2020-11-02T06:54:44.503816Z</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2021-10-05 14:33:03.261963</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://panelapp.agha.umccr.org/api/v1/panels/3149/?format=json</t>
         </is>
       </c>
     </row>

</xml_diff>